<commit_message>
Add Cases.xlxs and Check.xlsx
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -1,56 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nancygespens/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petrosovathur/Desktop/QA-Diplom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B700CE-5E1F-A54C-86C9-C452B9E0D0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC1950A-1E46-0544-B5E2-B4812527C9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="760" windowWidth="22160" windowHeight="17320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="v_1" sheetId="1" r:id="rId1"/>
+    <sheet name="Check_v1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="161">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>Группа проверок/модуль 
-(Test group/module)</t>
-  </si>
-  <si>
-    <t>Название (Title)</t>
-  </si>
-  <si>
-    <t>Приоритет (Priority)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Статус ручного теста 
-(Manual Test Status) </t>
-  </si>
-  <si>
-    <t>Результат ручного теста
-(Manual Test Result)</t>
-  </si>
-  <si>
-    <t>Статус авто-теста
-(Autotest Status)</t>
-  </si>
-  <si>
-    <t>Результат авто-теста
-(Autotest Result)</t>
-  </si>
-  <si>
     <t>Авторизация</t>
   </si>
   <si>
@@ -60,9 +34,6 @@
     <t>High</t>
   </si>
   <si>
-    <t>In Process</t>
-  </si>
-  <si>
     <t>Вход в личный кабинет с не валидными данными (латинские символы)</t>
   </si>
   <si>
@@ -328,13 +299,217 @@
   </si>
   <si>
     <t>Полнота информации цитат (в развернутом состоянии)</t>
+  </si>
+  <si>
+    <t>Блок/раздел</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>I1</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>K1</t>
+  </si>
+  <si>
+    <t>N4</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>Y2</t>
+  </si>
+  <si>
+    <t>Z1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>N1</t>
+  </si>
+  <si>
+    <t>O1</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>K2</t>
+  </si>
+  <si>
+    <t>N2</t>
+  </si>
+  <si>
+    <t>N3</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>V4</t>
+  </si>
+  <si>
+    <t>W1</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>Z2</t>
+  </si>
+  <si>
+    <t>Z3</t>
+  </si>
+  <si>
+    <t>AA1</t>
+  </si>
+  <si>
+    <t>AA2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -384,8 +559,37 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -394,60 +598,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE6B8AF"/>
-        <bgColor rgb="FFE6B8AF"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF4CCCC"/>
-        <bgColor rgb="FFF4CCCC"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFCE5CD"/>
-        <bgColor rgb="FFFCE5CD"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF2CC"/>
-        <bgColor rgb="FFFFF2CC"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD0E0E3"/>
-        <bgColor rgb="FFD0E0E3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC9DAF8"/>
-        <bgColor rgb="FFC9DAF8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCFE2F3"/>
-        <bgColor rgb="FFCFE2F3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9D2E9"/>
-        <bgColor rgb="FFD9D2E9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -456,717 +636,139 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="72">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB6D7A8"/>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1413,1189 +1015,1125 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I992"/>
+  <dimension ref="A1:H992"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" customWidth="1"/>
-    <col min="3" max="3" width="37.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" customWidth="1"/>
-    <col min="5" max="8" width="18.83203125" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" customWidth="1"/>
+    <col min="3" max="3" width="67" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" customWidth="1"/>
+    <col min="5" max="7" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="D2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="D3" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="D4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="D5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" s="10">
-        <v>44927</v>
-      </c>
-      <c r="B2" s="11" t="s">
+      <c r="D6" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D7" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="C8" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="C9" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="20"/>
-    </row>
-    <row r="3" spans="1:9" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A3" s="10">
-        <v>44958</v>
-      </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="13" t="s">
+      <c r="D9" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="20"/>
-    </row>
-    <row r="4" spans="1:9" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="10">
-        <v>44986</v>
-      </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="13" t="s">
+      <c r="D10" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="23"/>
+      <c r="C11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="20"/>
-    </row>
-    <row r="5" spans="1:9" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A5" s="10">
-        <v>45017</v>
-      </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="13" t="s">
+      <c r="D11" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" s="23"/>
+      <c r="C12" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="20"/>
-    </row>
-    <row r="6" spans="1:9" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A6" s="10">
-        <v>45047</v>
-      </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="13" t="s">
+      <c r="D12" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="20"/>
-    </row>
-    <row r="7" spans="1:9" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="10">
-        <v>45078</v>
-      </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="13" t="s">
+      <c r="D13" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="23"/>
+      <c r="C14" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-    </row>
-    <row r="8" spans="1:9" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A8" s="10">
-        <v>44928</v>
-      </c>
-      <c r="B8" s="15" t="s">
+      <c r="D14" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-    </row>
-    <row r="9" spans="1:9" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
-        <v>44929</v>
-      </c>
-      <c r="B9" s="11" t="s">
+      <c r="C15" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="D15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-    </row>
-    <row r="10" spans="1:9" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="14">
-        <v>44960</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="16" t="s">
+      <c r="D16" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:7" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17" s="23"/>
+      <c r="C17" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-    </row>
-    <row r="11" spans="1:9" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A11" s="14">
-        <v>44988</v>
-      </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="16" t="s">
+      <c r="D17" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-    </row>
-    <row r="12" spans="1:9" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" s="14">
-        <v>45019</v>
-      </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="16" t="s">
+      <c r="D18" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:7" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-    </row>
-    <row r="13" spans="1:9" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="14">
-        <v>45049</v>
-      </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="16" t="s">
+      <c r="D19" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="1:7" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B20" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-    </row>
-    <row r="14" spans="1:9" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="14">
-        <v>45080</v>
-      </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="16" t="s">
+      <c r="C20" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-    </row>
-    <row r="15" spans="1:9" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A15" s="10">
-        <v>44930</v>
-      </c>
-      <c r="B15" s="11" t="s">
+      <c r="D20" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21" spans="1:7" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B21" s="23"/>
+      <c r="C21" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="D21" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B22" s="23"/>
+      <c r="C22" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-    </row>
-    <row r="16" spans="1:9" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="10">
-        <v>44961</v>
-      </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="16" t="s">
+      <c r="D22" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+    </row>
+    <row r="23" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-    </row>
-    <row r="17" spans="1:8" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="10">
-        <v>44989</v>
-      </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="16" t="s">
+      <c r="C23" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-    </row>
-    <row r="18" spans="1:8" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="10">
-        <v>45020</v>
-      </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="16" t="s">
+      <c r="D23" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" spans="1:7" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-    </row>
-    <row r="19" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A19" s="10">
-        <v>45050</v>
-      </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="16" t="s">
+      <c r="C24" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-    </row>
-    <row r="20" spans="1:8" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="10">
-        <v>44931</v>
-      </c>
-      <c r="B20" s="17" t="s">
+      <c r="D24" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="1:7" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="23"/>
+      <c r="C25" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="D25" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+    </row>
+    <row r="26" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" s="23"/>
+      <c r="C26" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-    </row>
-    <row r="21" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A21" s="10">
-        <v>44962</v>
-      </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="16" t="s">
+      <c r="D26" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27" spans="1:7" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-    </row>
-    <row r="22" spans="1:8" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="10">
-        <v>44990</v>
-      </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="16" t="s">
+      <c r="C27" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-    </row>
-    <row r="23" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A23" s="10">
-        <v>44932</v>
-      </c>
-      <c r="B23" s="15" t="s">
+      <c r="D27" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+    </row>
+    <row r="28" spans="1:7" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28" s="23"/>
+      <c r="C28" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="D28" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+    </row>
+    <row r="29" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-    </row>
-    <row r="24" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A24" s="10">
-        <v>44933</v>
-      </c>
-      <c r="B24" s="11" t="s">
+      <c r="C29" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="D29" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+    </row>
+    <row r="30" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-    </row>
-    <row r="25" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A25" s="10">
-        <v>44964</v>
-      </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="16" t="s">
+      <c r="C30" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="14"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-    </row>
-    <row r="26" spans="1:8" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="10">
-        <v>44992</v>
-      </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="16" t="s">
+      <c r="D30" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" spans="1:7" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B31" s="23"/>
+      <c r="C31" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="14"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-    </row>
-    <row r="27" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A27" s="10">
-        <v>44934</v>
-      </c>
-      <c r="B27" s="11" t="s">
+      <c r="D31" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+    </row>
+    <row r="32" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B32" s="23"/>
+      <c r="C32" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="D32" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+    </row>
+    <row r="33" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B33" s="23"/>
+      <c r="C33" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="14"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-    </row>
-    <row r="28" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A28" s="10">
-        <v>44965</v>
-      </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="16" t="s">
+      <c r="D33" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+    </row>
+    <row r="34" spans="1:7" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="14"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-    </row>
-    <row r="29" spans="1:8" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A29" s="10">
-        <v>44935</v>
-      </c>
-      <c r="B29" s="15" t="s">
+      <c r="C34" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="D34" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+    </row>
+    <row r="35" spans="1:7" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B35" s="23"/>
+      <c r="C35" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="14"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-    </row>
-    <row r="30" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A30" s="10">
-        <v>44936</v>
-      </c>
-      <c r="B30" s="17" t="s">
+      <c r="D35" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+    </row>
+    <row r="36" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A36" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C36" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="14"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-    </row>
-    <row r="31" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A31" s="10">
-        <v>44967</v>
-      </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="16" t="s">
+      <c r="D36" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+    </row>
+    <row r="37" spans="1:7" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B37" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="14"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-    </row>
-    <row r="32" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A32" s="10">
-        <v>44995</v>
-      </c>
-      <c r="B32" s="23"/>
-      <c r="C32" s="16" t="s">
+      <c r="C37" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="14"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-    </row>
-    <row r="33" spans="1:8" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="10">
-        <v>45026</v>
-      </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="16" t="s">
+      <c r="D37" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+    </row>
+    <row r="38" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B38" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="14"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-    </row>
-    <row r="34" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A34" s="10">
-        <v>44937</v>
-      </c>
-      <c r="B34" s="11" t="s">
+      <c r="C38" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="D38" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+    </row>
+    <row r="39" spans="1:7" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B39" s="23"/>
+      <c r="C39" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="14"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-    </row>
-    <row r="35" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A35" s="10">
-        <v>44968</v>
-      </c>
-      <c r="B35" s="22"/>
-      <c r="C35" s="16" t="s">
+      <c r="D39" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+    </row>
+    <row r="40" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A40" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B40" s="23"/>
+      <c r="C40" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="14"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-    </row>
-    <row r="36" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A36" s="10">
-        <v>44938</v>
-      </c>
-      <c r="B36" s="15" t="s">
+      <c r="D40" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+    </row>
+    <row r="41" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A41" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B41" s="23"/>
+      <c r="C41" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="D41" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+    </row>
+    <row r="42" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A42" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B42" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D36" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="14"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-    </row>
-    <row r="37" spans="1:8" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="10">
-        <v>44939</v>
-      </c>
-      <c r="B37" s="18" t="s">
+      <c r="C42" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="D42" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+    </row>
+    <row r="43" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A43" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B43" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D37" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="14"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-    </row>
-    <row r="38" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A38" s="10">
-        <v>44940</v>
-      </c>
-      <c r="B38" s="11" t="s">
+      <c r="C43" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="D43" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+    </row>
+    <row r="44" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A44" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="D38" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="14"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-    </row>
-    <row r="39" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A39" s="10">
-        <v>44971</v>
-      </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="16" t="s">
+      <c r="C44" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D39" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="14"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-    </row>
-    <row r="40" spans="1:8" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="10">
-        <v>44999</v>
-      </c>
-      <c r="B40" s="21"/>
-      <c r="C40" s="16" t="s">
+      <c r="D44" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+    </row>
+    <row r="45" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A45" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B45" s="23"/>
+      <c r="C45" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="D40" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="14"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-    </row>
-    <row r="41" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A41" s="10">
-        <v>45030</v>
-      </c>
-      <c r="B41" s="22"/>
-      <c r="C41" s="16" t="s">
+      <c r="D45" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A46" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B46" s="23"/>
+      <c r="C46" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D41" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" s="14"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-    </row>
-    <row r="42" spans="1:8" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A42" s="10">
-        <v>44941</v>
-      </c>
-      <c r="B42" s="15" t="s">
+      <c r="D46" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+    </row>
+    <row r="47" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A47" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="B47" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="C47" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E42" s="14"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-    </row>
-    <row r="43" spans="1:8" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A43" s="10">
-        <v>44942</v>
-      </c>
-      <c r="B43" s="15" t="s">
+      <c r="D47" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+    </row>
+    <row r="48" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A48" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="B48" s="23"/>
+      <c r="C48" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="D48" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+    </row>
+    <row r="49" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A49" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B49" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D43" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="14"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
-    </row>
-    <row r="44" spans="1:8" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A44" s="10">
-        <v>44943</v>
-      </c>
-      <c r="B44" s="11" t="s">
+      <c r="C49" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="D49" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+    </row>
+    <row r="50" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A50" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B50" s="23"/>
+      <c r="C50" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D44" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E44" s="14"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="10"/>
-    </row>
-    <row r="45" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A45" s="10">
-        <v>44974</v>
-      </c>
-      <c r="B45" s="21"/>
-      <c r="C45" s="16" t="s">
+      <c r="D50" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+    </row>
+    <row r="51" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A51" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B51" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E45" s="14"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="10"/>
-    </row>
-    <row r="46" spans="1:8" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A46" s="10">
-        <v>45002</v>
-      </c>
-      <c r="B46" s="22"/>
-      <c r="C46" s="16" t="s">
+      <c r="C51" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="D46" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E46" s="14"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="10"/>
-    </row>
-    <row r="47" spans="1:8" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A47" s="10">
-        <v>44944</v>
-      </c>
-      <c r="B47" s="11" t="s">
+      <c r="D51" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+    </row>
+    <row r="52" spans="1:7" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B52" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C47" s="16" t="s">
+      <c r="C52" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D47" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E47" s="14"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
-    </row>
-    <row r="48" spans="1:8" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A48" s="10">
-        <v>44975</v>
-      </c>
-      <c r="B48" s="22"/>
-      <c r="C48" s="16" t="s">
+      <c r="D52" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+    </row>
+    <row r="53" spans="1:7" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B53" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="D48" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E48" s="14"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
-    </row>
-    <row r="49" spans="1:8" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A49" s="10">
-        <v>45003</v>
-      </c>
-      <c r="B49" s="11" t="s">
+      <c r="C53" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C49" s="16" t="s">
+      <c r="D53" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+    </row>
+    <row r="54" spans="1:7" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B54" s="23"/>
+      <c r="C54" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="D49" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E49" s="14"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
-      <c r="H49" s="10"/>
-    </row>
-    <row r="50" spans="1:8" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="10">
-        <v>45034</v>
-      </c>
-      <c r="B50" s="22"/>
-      <c r="C50" s="16" t="s">
+      <c r="D54" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+    </row>
+    <row r="55" spans="1:7" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B55" s="23"/>
+      <c r="C55" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="D50" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E50" s="14"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-    </row>
-    <row r="51" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A51" s="10">
-        <v>44945</v>
-      </c>
-      <c r="B51" s="15" t="s">
+      <c r="D55" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+    </row>
+    <row r="56" spans="1:7" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B56" s="23"/>
+      <c r="C56" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="C51" s="16" t="s">
+      <c r="D56" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+    </row>
+    <row r="57" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A57" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B57" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D51" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E51" s="14"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="10"/>
-      <c r="H51" s="10"/>
-    </row>
-    <row r="52" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A52" s="10">
-        <v>44946</v>
-      </c>
-      <c r="B52" s="15" t="s">
+      <c r="C57" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C52" s="16" t="s">
+      <c r="D57" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+    </row>
+    <row r="58" spans="1:7" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B58" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="D52" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E52" s="14"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
-    </row>
-    <row r="53" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A53" s="10">
-        <v>44947</v>
-      </c>
-      <c r="B53" s="11" t="s">
+      <c r="C58" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C53" s="16" t="s">
+      <c r="D58" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+    </row>
+    <row r="59" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A59" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B59" s="23"/>
+      <c r="C59" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D53" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E53" s="14"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-      <c r="H53" s="10"/>
-    </row>
-    <row r="54" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A54" s="10">
-        <v>44978</v>
-      </c>
-      <c r="B54" s="21"/>
-      <c r="C54" s="16" t="s">
+      <c r="D59" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+    </row>
+    <row r="60" spans="1:7" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B60" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="D54" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E54" s="14"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="10"/>
-      <c r="H54" s="10"/>
-    </row>
-    <row r="55" spans="1:8" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A55" s="10">
-        <v>45006</v>
-      </c>
-      <c r="B55" s="21"/>
-      <c r="C55" s="16" t="s">
+      <c r="C60" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="D55" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E55" s="14"/>
-      <c r="F55" s="10"/>
-      <c r="G55" s="10"/>
-      <c r="H55" s="10"/>
-    </row>
-    <row r="56" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A56" s="10">
-        <v>45037</v>
-      </c>
-      <c r="B56" s="22"/>
-      <c r="C56" s="16" t="s">
+      <c r="D60" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+    </row>
+    <row r="61" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A61" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B61" s="23"/>
+      <c r="C61" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="D56" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E56" s="14"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="10"/>
-      <c r="H56" s="10"/>
-    </row>
-    <row r="57" spans="1:8" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A57" s="10">
-        <v>44948</v>
-      </c>
-      <c r="B57" s="15" t="s">
+      <c r="D61" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+    </row>
+    <row r="62" spans="1:7" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B62" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="C62" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="D57" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E57" s="14"/>
-      <c r="F57" s="10"/>
-      <c r="G57" s="10"/>
-      <c r="H57" s="10"/>
-    </row>
-    <row r="58" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A58" s="10">
-        <v>44949</v>
-      </c>
-      <c r="B58" s="11" t="s">
+      <c r="D62" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+    </row>
+    <row r="63" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A63" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B63" s="23"/>
+      <c r="C63" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C58" s="16" t="s">
+      <c r="D63" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+    </row>
+    <row r="64" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A64" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B64" s="23"/>
+      <c r="C64" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="D58" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E58" s="14"/>
-      <c r="F58" s="10"/>
-      <c r="G58" s="10"/>
-      <c r="H58" s="10"/>
-    </row>
-    <row r="59" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A59" s="10">
-        <v>44980</v>
-      </c>
-      <c r="B59" s="22"/>
-      <c r="C59" s="16" t="s">
+      <c r="D64" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+    </row>
+    <row r="65" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A65" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B65" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="D59" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E59" s="14"/>
-      <c r="F59" s="10"/>
-      <c r="G59" s="10"/>
-      <c r="H59" s="10"/>
-    </row>
-    <row r="60" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A60" s="10">
-        <v>44950</v>
-      </c>
-      <c r="B60" s="11" t="s">
+      <c r="C65" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C60" s="16" t="s">
+      <c r="D65" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+    </row>
+    <row r="66" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A66" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="B66" s="23"/>
+      <c r="C66" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="D60" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E60" s="14"/>
-      <c r="F60" s="10"/>
-      <c r="G60" s="10"/>
-      <c r="H60" s="10"/>
-    </row>
-    <row r="61" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A61" s="10">
-        <v>44981</v>
-      </c>
-      <c r="B61" s="22"/>
-      <c r="C61" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="D61" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E61" s="14"/>
-      <c r="F61" s="10"/>
-      <c r="G61" s="10"/>
-      <c r="H61" s="10"/>
-    </row>
-    <row r="62" spans="1:8" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A62" s="10">
-        <v>44951</v>
-      </c>
-      <c r="B62" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C62" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="D62" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E62" s="14"/>
-      <c r="F62" s="10"/>
-      <c r="G62" s="10"/>
-      <c r="H62" s="10"/>
-    </row>
-    <row r="63" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A63" s="10">
-        <v>44982</v>
-      </c>
-      <c r="B63" s="21"/>
-      <c r="C63" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E63" s="14"/>
-      <c r="F63" s="10"/>
-      <c r="G63" s="10"/>
-      <c r="H63" s="10"/>
-    </row>
-    <row r="64" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A64" s="10">
-        <v>45010</v>
-      </c>
-      <c r="B64" s="22"/>
-      <c r="C64" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="D64" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E64" s="14"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="10"/>
-      <c r="H64" s="10"/>
-    </row>
-    <row r="65" spans="1:8" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A65" s="10">
-        <v>44952</v>
-      </c>
-      <c r="B65" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C65" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D65" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E65" s="14"/>
-      <c r="F65" s="10"/>
-      <c r="G65" s="10"/>
-      <c r="H65" s="10"/>
-    </row>
-    <row r="66" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A66" s="10">
-        <v>44983</v>
-      </c>
-      <c r="B66" s="22"/>
-      <c r="C66" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="D66" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E66" s="14"/>
-      <c r="F66" s="10"/>
-      <c r="G66" s="10"/>
-      <c r="H66" s="10"/>
-    </row>
-    <row r="67" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="B67" s="1"/>
-    </row>
-    <row r="68" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="B68" s="1"/>
-    </row>
-    <row r="69" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="B69" s="1"/>
-    </row>
-    <row r="70" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="B70" s="1"/>
-    </row>
-    <row r="71" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="D66" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+    </row>
+    <row r="67" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="7"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+    </row>
+    <row r="68" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A68" s="7"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+    </row>
+    <row r="69" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+      <c r="A69" s="7"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="7"/>
+    </row>
+    <row r="70" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+      <c r="A70" s="7"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="7"/>
+    </row>
+    <row r="71" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="B71" s="1"/>
     </row>
-    <row r="72" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="B72" s="1"/>
     </row>
-    <row r="73" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="B73" s="1"/>
     </row>
-    <row r="74" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="B74" s="1"/>
     </row>
-    <row r="75" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="B75" s="1"/>
     </row>
-    <row r="76" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="B76" s="1"/>
     </row>
-    <row r="77" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="B77" s="1"/>
     </row>
-    <row r="78" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="B78" s="1"/>
     </row>
-    <row r="79" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="B79" s="1"/>
     </row>
-    <row r="80" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="B80" s="1"/>
     </row>
     <row r="81" spans="2:2" ht="13" x14ac:dyDescent="0.15">
@@ -5348,384 +4886,38 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="B53:B56"/>
     <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B2:B7"/>
     <mergeCell ref="B9:B14"/>
     <mergeCell ref="B15:B19"/>
     <mergeCell ref="B20:B22"/>
     <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B2:B7"/>
   </mergeCells>
-  <conditionalFormatting sqref="H37">
-    <cfRule type="cellIs" dxfId="71" priority="1" operator="equal">
+  <phoneticPr fontId="10" type="noConversion"/>
+  <conditionalFormatting sqref="E2:E37">
+    <cfRule type="cellIs" dxfId="3" priority="37" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H37">
-    <cfRule type="cellIs" dxfId="70" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="38" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
-    <cfRule type="cellIs" dxfId="69" priority="3" operator="equal">
+  <conditionalFormatting sqref="G2:G37">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
-    <cfRule type="cellIs" dxfId="68" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="67" priority="5" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="66" priority="6" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="65" priority="7" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="64" priority="8" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H30:H33">
-    <cfRule type="cellIs" dxfId="63" priority="9" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H30:H33">
-    <cfRule type="cellIs" dxfId="62" priority="10" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="61" priority="11" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="60" priority="12" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H28">
-    <cfRule type="cellIs" dxfId="59" priority="13" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H28">
-    <cfRule type="cellIs" dxfId="58" priority="14" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="57" priority="15" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="56" priority="16" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="55" priority="17" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="54" priority="18" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="53" priority="19" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="52" priority="20" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="51" priority="21" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="50" priority="22" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H22:H23">
-    <cfRule type="cellIs" dxfId="49" priority="23" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H22:H23">
-    <cfRule type="cellIs" dxfId="48" priority="24" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15:H21">
-    <cfRule type="cellIs" dxfId="47" priority="25" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15:H21">
-    <cfRule type="cellIs" dxfId="46" priority="26" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H12:H14">
-    <cfRule type="cellIs" dxfId="45" priority="27" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H12:H14">
-    <cfRule type="cellIs" dxfId="44" priority="28" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10:H11">
-    <cfRule type="cellIs" dxfId="43" priority="29" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10:H11">
-    <cfRule type="cellIs" dxfId="42" priority="30" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="41" priority="31" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="40" priority="32" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H7:H8">
-    <cfRule type="cellIs" dxfId="39" priority="33" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H7:H8">
-    <cfRule type="cellIs" dxfId="38" priority="34" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H6">
-    <cfRule type="cellIs" dxfId="37" priority="35" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H6">
-    <cfRule type="cellIs" dxfId="36" priority="36" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F37">
-    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F37">
-    <cfRule type="cellIs" dxfId="34" priority="38" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F36">
-    <cfRule type="cellIs" dxfId="33" priority="39" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F36">
-    <cfRule type="cellIs" dxfId="32" priority="40" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F35">
-    <cfRule type="cellIs" dxfId="31" priority="41" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F35">
-    <cfRule type="cellIs" dxfId="30" priority="42" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F34">
-    <cfRule type="cellIs" dxfId="29" priority="43" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F34">
-    <cfRule type="cellIs" dxfId="28" priority="44" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F30:F33">
-    <cfRule type="cellIs" dxfId="27" priority="45" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F30:F33">
-    <cfRule type="cellIs" dxfId="26" priority="46" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F29">
-    <cfRule type="cellIs" dxfId="25" priority="47" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F29">
-    <cfRule type="cellIs" dxfId="24" priority="48" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="23" priority="49" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="22" priority="50" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F27">
-    <cfRule type="cellIs" dxfId="21" priority="51" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F27">
-    <cfRule type="cellIs" dxfId="20" priority="52" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F26">
-    <cfRule type="cellIs" dxfId="19" priority="53" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F26">
-    <cfRule type="cellIs" dxfId="18" priority="54" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F25">
-    <cfRule type="cellIs" dxfId="17" priority="55" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F25">
-    <cfRule type="cellIs" dxfId="16" priority="56" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F24">
-    <cfRule type="cellIs" dxfId="15" priority="57" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F24">
-    <cfRule type="cellIs" dxfId="14" priority="58" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F22:F23">
-    <cfRule type="cellIs" dxfId="13" priority="59" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F22:F23">
-    <cfRule type="cellIs" dxfId="12" priority="60" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F15:F21">
-    <cfRule type="cellIs" dxfId="11" priority="61" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F15:F21">
-    <cfRule type="cellIs" dxfId="10" priority="62" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12:F14">
-    <cfRule type="cellIs" dxfId="9" priority="63" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12:F14">
-    <cfRule type="cellIs" dxfId="8" priority="64" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10:F11">
-    <cfRule type="cellIs" dxfId="7" priority="65" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10:F11">
-    <cfRule type="cellIs" dxfId="6" priority="66" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="5" priority="67" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="4" priority="68" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F7:F8">
-    <cfRule type="cellIs" dxfId="3" priority="69" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F7:F8">
-    <cfRule type="cellIs" dxfId="2" priority="70" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F6">
-    <cfRule type="cellIs" dxfId="1" priority="71" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F6">
-    <cfRule type="cellIs" dxfId="0" priority="72" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" sqref="D2:D66" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D66" xr:uid="{11A53942-531C-744B-8306-914430C1FA4A}">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F66 H2:H66" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="E2:E66 G2:G66" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Passed,Failed,No Result"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G2:G66" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F66" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"In process,Done,Need to update"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E2:E66" xr:uid="{00000000-0002-0000-0000-000003000000}">
-      <formula1>"In Process,Done,Need to update"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>